<commit_message>
Updated mappings following refactoring of atmos_solar and atmos_volcanos to make atmos_natural_forcing
</commit_message>
<xml_diff>
--- a/mappings/atmos-cmip5-to-cmip6-property-mappings.xlsx
+++ b/mappings/atmos-cmip5-to-cmip6-property-mappings.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-atmos/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="27840" yWindow="1100" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -407,30 +402,6 @@
     <t>CMIP6 Specialization ID</t>
   </si>
   <si>
-    <t>cmip6.atmos.solar.orbital_parameters.computation_method</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.orbital_parameters.fixed_reference_date</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.orbital_parameters.type</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.solar_constant.fixed_value</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.orbital_parameters.transient_method</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.solar_constant.transient_characteristics</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.solar.solar_constant.type</t>
-  </si>
-  <si>
-    <t>cmip6.atmos.volcanos.volcanoes_treatment.volcanoes_implementation</t>
-  </si>
-  <si>
     <t>cmip6.atmos.turbulence_convection.boundary_layer_turbulence.closure_order</t>
   </si>
   <si>
@@ -560,9 +531,6 @@
     <t>cmip6.atmos.radiation.shortwave_radiation.spectral_integration</t>
   </si>
   <si>
-    <t>cmip6.atmos.solar.insolation_ozone.solar_ozone_impact</t>
-  </si>
-  <si>
     <t>cmip6.atmos.microphysics_precipitation.large_scale_cloud_microphysics.scheme_name</t>
   </si>
   <si>
@@ -572,9 +540,6 @@
     <t>cmip6.atmos.cloud_scheme.optical_cloud_properties.cloud_overlap_method</t>
   </si>
   <si>
-    <t>cmip6.atmos.cloud_scheme.prognostic_scheme</t>
-  </si>
-  <si>
     <t>cmip6.atmos.observation_simulation.cosp_attributes.run_configuration</t>
   </si>
   <si>
@@ -645,6 +610,36 @@
   </si>
   <si>
     <t>cmip6.atmos.dynamical_core.advection.tracers.scheme_name</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.insolation_ozone.solar_ozone_impact</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.orbital_parameters.computation_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.orbital_parameters.fixed_reference_date</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.orbital_parameters.transient_method</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.orbital_parameters.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.solar_constant.fixed_value</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.solar_constant.transient_characteristics</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.solar_constant.type</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.natural_forcing.volcanoes_treatment.volcanoes_implementation</t>
+  </si>
+  <si>
+    <t>cmip6.atmos.cloud_scheme.scheme_type</t>
   </si>
 </sst>
 </file>
@@ -2313,11 +2308,11 @@
   </sheetPr>
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2325,7 +2320,7 @@
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>123</v>
       </c>
@@ -2336,7 +2331,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>122</v>
       </c>
@@ -2344,10 +2339,10 @@
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>122</v>
       </c>
@@ -2355,10 +2350,10 @@
         <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>122</v>
       </c>
@@ -2369,7 +2364,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>122</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>122</v>
       </c>
@@ -2388,10 +2383,10 @@
         <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>122</v>
       </c>
@@ -2399,10 +2394,10 @@
         <v>107</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>122</v>
       </c>
@@ -2410,10 +2405,10 @@
         <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>122</v>
       </c>
@@ -2422,7 +2417,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>122</v>
       </c>
@@ -2431,7 +2426,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>122</v>
       </c>
@@ -2439,10 +2434,10 @@
         <v>111</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>122</v>
       </c>
@@ -2450,10 +2445,10 @@
         <v>112</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>122</v>
       </c>
@@ -2461,10 +2456,10 @@
         <v>113</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>122</v>
       </c>
@@ -2473,7 +2468,7 @@
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>122</v>
       </c>
@@ -2481,10 +2476,10 @@
         <v>115</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>122</v>
       </c>
@@ -2492,10 +2487,10 @@
         <v>116</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>122</v>
       </c>
@@ -2503,10 +2498,10 @@
         <v>117</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -2514,10 +2509,10 @@
         <v>118</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>122</v>
       </c>
@@ -2525,10 +2520,10 @@
         <v>119</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>122</v>
       </c>
@@ -2537,7 +2532,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>122</v>
       </c>
@@ -2546,12 +2541,12 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="20" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="20.25" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -2559,10 +2554,10 @@
         <v>7</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="20.25" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -2570,10 +2565,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20.25" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -2581,10 +2576,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.25" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2592,10 +2587,10 @@
         <v>10</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.25" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2603,7 +2598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="20.25" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2611,10 +2606,10 @@
         <v>12</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.25" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2622,10 +2617,10 @@
         <v>13</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.25" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2633,10 +2628,10 @@
         <v>14</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.25" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2644,10 +2639,10 @@
         <v>15</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.25" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2655,10 +2650,10 @@
         <v>16</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.25" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2666,10 +2661,10 @@
         <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.25" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2677,10 +2672,10 @@
         <v>18</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -2688,10 +2683,10 @@
         <v>19</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2695,7 @@
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="20.25" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2709,7 +2704,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -2717,10 +2712,10 @@
         <v>22</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -2728,10 +2723,10 @@
         <v>23</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
@@ -2739,15 +2734,15 @@
         <v>24</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>1</v>
       </c>
@@ -2755,10 +2750,10 @@
         <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2767,7 +2762,7 @@
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
@@ -2778,7 +2773,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -2786,10 +2781,10 @@
         <v>28</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>1</v>
       </c>
@@ -2797,10 +2792,10 @@
         <v>29</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
@@ -2811,7 +2806,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
@@ -2822,7 +2817,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
@@ -2833,7 +2828,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2844,12 +2839,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2857,10 +2852,10 @@
         <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2868,10 +2863,10 @@
         <v>35</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -2879,10 +2874,10 @@
         <v>36</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2890,10 +2885,10 @@
         <v>37</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2901,10 +2896,10 @@
         <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -2912,10 +2907,10 @@
         <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
@@ -2923,10 +2918,10 @@
         <v>40</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -2934,10 +2929,10 @@
         <v>41</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -2945,10 +2940,10 @@
         <v>42</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -2956,10 +2951,10 @@
         <v>43</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -2967,10 +2962,10 @@
         <v>44</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -2978,15 +2973,15 @@
         <v>45</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="2"/>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
@@ -2994,10 +2989,10 @@
         <v>46</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
@@ -3005,10 +3000,10 @@
         <v>47</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
@@ -3016,10 +3011,10 @@
         <v>48</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -3027,10 +3022,10 @@
         <v>49</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
@@ -3038,10 +3033,10 @@
         <v>50</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -3049,10 +3044,10 @@
         <v>51</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -3060,10 +3055,10 @@
         <v>52</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
@@ -3071,10 +3066,10 @@
         <v>53</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
@@ -3082,10 +3077,10 @@
         <v>54</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>3</v>
       </c>
@@ -3093,10 +3088,10 @@
         <v>55</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>3</v>
       </c>
@@ -3104,10 +3099,10 @@
         <v>56</v>
       </c>
       <c r="C75" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -3115,10 +3110,10 @@
         <v>57</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -3126,15 +3121,15 @@
         <v>58</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="2"/>
       <c r="B78" s="3"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>4</v>
       </c>
@@ -3142,10 +3137,10 @@
         <v>59</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>4</v>
       </c>
@@ -3153,10 +3148,10 @@
         <v>60</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
@@ -3164,10 +3159,10 @@
         <v>61</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>4</v>
       </c>
@@ -3175,10 +3170,10 @@
         <v>62</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3182,7 @@
       </c>
       <c r="C83" s="4"/>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>4</v>
       </c>
@@ -3195,15 +3190,15 @@
         <v>64</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="2"/>
       <c r="B85" s="3"/>
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>4</v>
       </c>
@@ -3211,10 +3206,10 @@
         <v>65</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="2" t="s">
         <v>4</v>
       </c>
@@ -3222,10 +3217,10 @@
         <v>66</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>4</v>
       </c>
@@ -3233,10 +3228,10 @@
         <v>67</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>4</v>
       </c>
@@ -3244,15 +3239,15 @@
         <v>68</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="20.25" customHeight="1">
       <c r="A90" s="2"/>
       <c r="B90" s="3"/>
       <c r="C90" s="4"/>
     </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -3260,10 +3255,10 @@
         <v>69</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="20.25" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -3272,7 +3267,7 @@
       </c>
       <c r="C92" s="4"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -3281,7 +3276,7 @@
       </c>
       <c r="C93" s="4"/>
     </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -3289,10 +3284,10 @@
         <v>72</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -3300,10 +3295,10 @@
         <v>73</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -3311,10 +3306,10 @@
         <v>74</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -3322,10 +3317,10 @@
         <v>75</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -3333,10 +3328,10 @@
         <v>76</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="20.25" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -3345,7 +3340,7 @@
       </c>
       <c r="C99" s="4"/>
     </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -3353,10 +3348,10 @@
         <v>78</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -3364,10 +3359,10 @@
         <v>79</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -3375,10 +3370,10 @@
         <v>80</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -3386,10 +3381,10 @@
         <v>81</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
@@ -3397,15 +3392,15 @@
         <v>82</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="20.25" customHeight="1">
       <c r="A105" s="2"/>
       <c r="B105" s="3"/>
       <c r="C105" s="4"/>
     </row>
-    <row r="106" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:3" ht="20.25" customHeight="1">
       <c r="A106" s="2" t="s">
         <v>6</v>
       </c>
@@ -3413,10 +3408,10 @@
         <v>83</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="20.25" customHeight="1">
       <c r="A107" s="2" t="s">
         <v>6</v>
       </c>
@@ -3425,7 +3420,7 @@
       </c>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:3" ht="20.25" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>6</v>
       </c>
@@ -3434,7 +3429,7 @@
       </c>
       <c r="C108" s="4"/>
     </row>
-    <row r="109" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:3" ht="20.25" customHeight="1">
       <c r="A109" s="2" t="s">
         <v>6</v>
       </c>
@@ -3443,7 +3438,7 @@
       </c>
       <c r="C109"/>
     </row>
-    <row r="110" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:3" ht="20.25" customHeight="1">
       <c r="A110" s="2" t="s">
         <v>6</v>
       </c>
@@ -3451,10 +3446,10 @@
         <v>87</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="20.25" customHeight="1">
       <c r="A111" s="2" t="s">
         <v>6</v>
       </c>
@@ -3462,10 +3457,10 @@
         <v>88</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="20.25" customHeight="1">
       <c r="A112" s="2" t="s">
         <v>6</v>
       </c>
@@ -3473,10 +3468,10 @@
         <v>89</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="20.25" customHeight="1">
       <c r="A113" s="2" t="s">
         <v>6</v>
       </c>
@@ -3485,7 +3480,7 @@
       </c>
       <c r="C113" s="4"/>
     </row>
-    <row r="114" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:3" ht="20.25" customHeight="1">
       <c r="A114" s="2" t="s">
         <v>6</v>
       </c>
@@ -3493,10 +3488,10 @@
         <v>91</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="20.25" customHeight="1">
       <c r="A115" s="2" t="s">
         <v>6</v>
       </c>
@@ -3504,10 +3499,10 @@
         <v>92</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="20.25" customHeight="1">
       <c r="A116" s="2" t="s">
         <v>6</v>
       </c>
@@ -3516,7 +3511,7 @@
       </c>
       <c r="C116" s="4"/>
     </row>
-    <row r="117" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:3" ht="20.25" customHeight="1">
       <c r="A117" s="2" t="s">
         <v>6</v>
       </c>
@@ -3531,5 +3526,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>